<commit_message>
fixing template and code repair
</commit_message>
<xml_diff>
--- a/Projects/SINGHATH/Data/Template.xlsx
+++ b/Projects/SINGHATH/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,18 +23,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="43">
-  <si>
-    <t xml:space="preserve">kpi_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">store_types</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sheet name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">is_active</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
+  <si>
+    <t xml:space="preserve">KPI_NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STORE_TYPES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHEET_NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IS_ACTIVE</t>
   </si>
   <si>
     <t xml:space="preserve">SIMON_PRICE_DIFFERENCE</t>
@@ -112,6 +112,18 @@
     <t xml:space="preserve">POS EAN CODE</t>
   </si>
   <si>
+    <t xml:space="preserve">Price tag of Singha water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POS01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price tag of Leo beer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POS02</t>
+  </si>
+  <si>
     <t xml:space="preserve">CATEGORY</t>
   </si>
   <si>
@@ -142,16 +154,13 @@
     <t xml:space="preserve">AND</t>
   </si>
   <si>
+    <t xml:space="preserve">POS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">beer_dump</t>
+  </si>
+  <si>
     <t xml:space="preserve">Other</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EAN 00018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">beer_dump</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EAN 00016</t>
   </si>
 </sst>
 </file>
@@ -441,14 +450,14 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="41.8825910931174"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="42.2064777327935"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="42.2064777327935"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="42.5263157894737"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="29.3522267206478"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="2" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.10526315789474"/>
   </cols>
@@ -527,19 +536,19 @@
   </sheetPr>
   <dimension ref="1:6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="36.8502024291498"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="33.8502024291498"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="29.3522267206478"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="36.8502024291498"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="11" width="36.8502024291498"/>
-    <col collapsed="false" hidden="false" max="1018" min="6" style="12" width="36.8502024291498"/>
-    <col collapsed="false" hidden="false" max="1025" min="1019" style="13" width="36.8502024291498"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="37.17004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="34.17004048583"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="37.17004048583"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="11" width="37.17004048583"/>
+    <col collapsed="false" hidden="false" max="1018" min="6" style="12" width="37.17004048583"/>
+    <col collapsed="false" hidden="false" max="1025" min="1019" style="13" width="37.17004048583"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -619,7 +628,7 @@
         <v>20</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" s="13"/>
       <c r="K3" s="0"/>
@@ -628,7 +637,7 @@
       <c r="N3" s="0"/>
       <c r="O3" s="0"/>
     </row>
-    <row r="4" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="n">
         <v>8850999009674</v>
       </c>
@@ -642,7 +651,7 @@
         <v>22</v>
       </c>
       <c r="E4" s="11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K4" s="0"/>
       <c r="L4" s="0"/>
@@ -650,7 +659,7 @@
       <c r="N4" s="0"/>
       <c r="O4" s="0"/>
     </row>
-    <row r="5" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="n">
         <v>8850999171401</v>
       </c>
@@ -667,7 +676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="n">
         <v>8850999141008</v>
       </c>
@@ -681,7 +690,7 @@
         <v>26</v>
       </c>
       <c r="E6" s="11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -704,16 +713,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:5"/>
+  <dimension ref="1:3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K26" activeCellId="0" sqref="K26"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="34.4939271255061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="34.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.7449392712551"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -728,34 +737,18 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="1" t="n">
-        <v>8850999143002</v>
+        <v>29</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>8851993613010</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="1" t="n">
-        <v>8851993616011</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="1" t="n">
-        <v>8851993623019</v>
+        <v>31</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -776,119 +769,119 @@
   </sheetPr>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="3" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="20" width="10.8178137651822"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="21" width="61.5951417004049"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="21" width="62.1295546558704"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="21" width="8.89068825910931"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="12.9595141700405"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="3" width="6.21457489878543"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="14" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C2" s="21" t="n">
         <v>8850999321028</v>
       </c>
       <c r="D2" s="21" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>40</v>
+        <v>43</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>30</v>
       </c>
       <c r="D3" s="21" t="n">
         <v>1</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C4" s="21" t="n">
         <v>8850999143026</v>
       </c>
       <c r="D4" s="21" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="22" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="D5" s="21" t="n">
         <v>1</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F5" s="22" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed dump display presence
</commit_message>
<xml_diff>
--- a/Projects/SINGHATH/Data/Template.xlsx
+++ b/Projects/SINGHATH/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
   <si>
     <t xml:space="preserve">KPI_NAME</t>
   </si>
@@ -148,6 +148,9 @@
     <t xml:space="preserve">SKU</t>
   </si>
   <si>
+    <t xml:space="preserve">8850999321028,8850999320021,8850999321004,8850999320007</t>
+  </si>
+  <si>
     <t xml:space="preserve">Stacks</t>
   </si>
   <si>
@@ -158,6 +161,9 @@
   </si>
   <si>
     <t xml:space="preserve">beer_dump</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8850999143026,8850999141015,8850999009681,8850999171364</t>
   </si>
   <si>
     <t xml:space="preserve">Other</t>
@@ -167,10 +173,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0"/>
+    <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -192,6 +200,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -222,7 +237,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF3333"/>
-        <bgColor rgb="FFFF6600"/>
+        <bgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
     <fill>
@@ -273,7 +288,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -314,6 +329,10 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -342,6 +361,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -354,6 +377,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -362,12 +389,32 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -383,7 +430,7 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF3333"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -426,7 +473,7 @@
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FFFF3333"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
@@ -453,16 +500,16 @@
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="42.2064777327935"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="42.5263157894737"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="29.3522267206478"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="42.9554655870445"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="43.3846153846154"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="29.7773279352227"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="2" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="5" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -476,7 +523,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
@@ -490,7 +537,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
@@ -504,7 +551,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
@@ -534,79 +581,79 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:6"/>
+  <dimension ref="1:7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="37.17004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="34.17004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="29.5668016194332"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="37.17004048583"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="11" width="37.17004048583"/>
-    <col collapsed="false" hidden="false" max="1018" min="6" style="12" width="37.17004048583"/>
-    <col collapsed="false" hidden="false" max="1025" min="1019" style="13" width="37.17004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="37.7044534412955"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="34.7085020242915"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="11" width="37.7044534412955"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="12" width="37.7044534412955"/>
+    <col collapsed="false" hidden="false" max="1018" min="6" style="13" width="37.7044534412955"/>
+    <col collapsed="false" hidden="false" max="1025" min="1019" style="14" width="37.7044534412955"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="14" t="s">
+    <row r="1" s="5" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="14"/>
-      <c r="E1" s="15"/>
-    </row>
-    <row r="2" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="16" t="s">
+      <c r="D1" s="15"/>
+      <c r="E1" s="16"/>
+    </row>
+    <row r="2" s="21" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="19" t="s">
         <v>18</v>
       </c>
       <c r="F2" s="5"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="18"/>
-      <c r="R2" s="18"/>
-      <c r="S2" s="18"/>
-      <c r="T2" s="18"/>
-      <c r="U2" s="18"/>
-      <c r="V2" s="18"/>
-      <c r="W2" s="18"/>
-      <c r="X2" s="18"/>
-      <c r="Y2" s="18"/>
-      <c r="Z2" s="18"/>
-      <c r="AA2" s="18"/>
-      <c r="AB2" s="18"/>
-      <c r="AC2" s="18"/>
-      <c r="AD2" s="18"/>
-      <c r="AE2" s="18"/>
-      <c r="AF2" s="18"/>
-      <c r="AG2" s="18"/>
-      <c r="AH2" s="18"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="20"/>
+      <c r="V2" s="20"/>
+      <c r="W2" s="20"/>
+      <c r="X2" s="20"/>
+      <c r="Y2" s="20"/>
+      <c r="Z2" s="20"/>
+      <c r="AA2" s="20"/>
+      <c r="AB2" s="20"/>
+      <c r="AC2" s="20"/>
+      <c r="AD2" s="20"/>
+      <c r="AE2" s="20"/>
+      <c r="AF2" s="20"/>
+      <c r="AG2" s="20"/>
+      <c r="AH2" s="20"/>
       <c r="AME2" s="5"/>
       <c r="AMF2" s="5"/>
       <c r="AMG2" s="5"/>
@@ -621,7 +668,7 @@
       <c r="B3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="C3" s="22" t="n">
         <v>8851993623019</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -630,14 +677,9 @@
       <c r="E3" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F3" s="13"/>
-      <c r="K3" s="0"/>
-      <c r="L3" s="0"/>
-      <c r="M3" s="0"/>
-      <c r="N3" s="0"/>
-      <c r="O3" s="0"/>
-    </row>
-    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="n">
         <v>8850999009674</v>
       </c>
@@ -647,19 +689,14 @@
       <c r="C4" s="10" t="n">
         <v>8851993625013</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="11" t="n">
+      <c r="E4" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="K4" s="0"/>
-      <c r="L4" s="0"/>
-      <c r="M4" s="0"/>
-      <c r="N4" s="0"/>
-      <c r="O4" s="0"/>
-    </row>
-    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="5" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="n">
         <v>8850999171401</v>
       </c>
@@ -669,14 +706,14 @@
       <c r="C5" s="10" t="n">
         <v>8851993613010</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="11" t="n">
+      <c r="E5" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="n">
         <v>8850999141008</v>
       </c>
@@ -686,13 +723,18 @@
       <c r="C6" s="10" t="n">
         <v>8851993616011</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="11" t="n">
+      <c r="E6" s="12" t="n">
         <v>2</v>
       </c>
     </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
@@ -713,29 +755,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="34.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="35.1336032388664"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.9595141700405"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="5" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AMJ1" s="0"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>29</v>
       </c>
@@ -743,7 +784,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
@@ -769,119 +810,119 @@
   </sheetPr>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="3" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="10.8178137651822"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="21" width="62.1295546558704"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="8.89068825910931"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="23" width="10.8178137651822"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="24" width="73.5910931174089"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="24" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="13.1740890688259"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="3" width="6.21457489878543"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="14" t="s">
+    <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="15" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22" t="s">
+    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="21" t="n">
-        <v>8850999321028</v>
-      </c>
-      <c r="D2" s="21" t="n">
+      <c r="C2" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="24" t="n">
         <v>12</v>
       </c>
-      <c r="E2" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" s="22" t="s">
+      <c r="E2" s="29" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="22" t="s">
+      <c r="F2" s="29" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="21" t="n">
+    </row>
+    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="24" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="29" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="24" t="n">
         <v>1</v>
       </c>
-      <c r="E3" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="F3" s="22" t="s">
+      <c r="E5" s="29" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="21" t="n">
-        <v>8850999143026</v>
-      </c>
-      <c r="D4" s="21" t="n">
-        <v>3</v>
-      </c>
-      <c r="E4" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" s="22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="F5" s="22" t="s">
-        <v>42</v>
+      <c r="F5" s="29" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixing beer dump display
</commit_message>
<xml_diff>
--- a/Projects/SINGHATH/Data/Template.xlsx
+++ b/Projects/SINGHATH/Data/Template.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Price" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="POS Presence" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Dump Display Presence" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Notes While Filling Template" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="50">
   <si>
     <t xml:space="preserve">KPI_NAME</t>
   </si>
@@ -148,25 +149,98 @@
     <t xml:space="preserve">SKU</t>
   </si>
   <si>
-    <t xml:space="preserve">8850999321028,8850999320021,8850999321004,8850999320007</t>
+    <t xml:space="preserve">8850999321004,8850999320007</t>
   </si>
   <si>
     <t xml:space="preserve">Stacks</t>
   </si>
   <si>
+    <t xml:space="preserve">OR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8850999320021,8850999321028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POS</t>
+  </si>
+  <si>
     <t xml:space="preserve">AND</t>
   </si>
   <si>
-    <t xml:space="preserve">POS</t>
-  </si>
-  <si>
     <t xml:space="preserve">beer_dump</t>
   </si>
   <si>
     <t xml:space="preserve">8850999143026,8850999141015,8850999009681,8850999171364</t>
   </si>
   <si>
-    <t xml:space="preserve">Other</t>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">LOGIC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">: The OR LOGIC rows will be grouped and checked if either any of them passses. Then it is ANDed with the POS row. 
+Also, the LOGIC per PROD_TYPE needs to be same.
+Example, for SKU in water_dump, the LOGIC must be OR for all rows.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">SCENE_TYPE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">: The scene_type for a single category is expected to be </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">uniform</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.
+Example, for water_dump, all rows are expected to be of SCENE_TYPE as `Stacks`.
+DUMP DISPLAY PRESENCE is expected to have both POS and SKU</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -178,7 +252,7 @@
     <numFmt numFmtId="165" formatCode="0"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -202,14 +276,23 @@
       <family val="0"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -237,7 +320,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF3333"/>
-        <bgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF6600"/>
       </patternFill>
     </fill>
     <fill>
@@ -246,8 +329,20 @@
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF99FF"/>
+        <bgColor rgb="FFCC99FF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -260,6 +355,13 @@
       <right style="hair"/>
       <top style="hair"/>
       <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -288,7 +390,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -381,40 +483,52 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -430,7 +544,7 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFFF3333"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -465,7 +579,7 @@
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFFF99FF"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
@@ -473,7 +587,7 @@
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF3333"/>
+      <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
@@ -496,15 +610,15 @@
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="42.9554655870445"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="43.3846153846154"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="29.7773279352227"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="45.417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="45.8461538461538"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="31.4939271255061"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="2" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.10526315789474"/>
   </cols>
@@ -583,19 +697,19 @@
   </sheetPr>
   <dimension ref="1:7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="37.7044534412955"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="34.7085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="28.7085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="11" width="37.7044534412955"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="12" width="37.7044534412955"/>
-    <col collapsed="false" hidden="false" max="1018" min="6" style="13" width="37.7044534412955"/>
-    <col collapsed="false" hidden="false" max="1025" min="1019" style="14" width="37.7044534412955"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="39.8502024291498"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="36.5263157894737"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="30.2064777327935"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="11" width="39.8502024291498"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="12" width="39.8502024291498"/>
+    <col collapsed="false" hidden="false" max="1018" min="6" style="13" width="39.8502024291498"/>
+    <col collapsed="false" hidden="false" max="1025" min="1019" style="14" width="39.8502024291498"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -757,14 +871,14 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="35.1336032388664"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="37.17004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -808,31 +922,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="23" width="10.8178137651822"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="24" width="73.5910931174089"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="24" width="8.89068825910931"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="6.21457489878543"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="24" width="10.8178137651822"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="25" width="78.0890688259109"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="25" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="23" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="23" width="6.21457489878543"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="15" t="s">
         <v>35</v>
       </c>
       <c r="D1" s="15" t="s">
@@ -845,7 +959,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="26" t="s">
         <v>39</v>
       </c>
@@ -855,74 +969,94 @@
       <c r="C2" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="24" t="n">
+      <c r="D2" s="29" t="n">
         <v>12</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="F2" s="26" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="29" t="s">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="D3" s="29" t="n">
+        <v>3</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="24" t="n">
+      <c r="D4" s="29" t="n">
         <v>1</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="E4" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="29" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="26" t="s">
+      <c r="F4" s="26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="33" t="n">
+        <v>3</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="28" t="s">
+      <c r="C6" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="33" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="30" t="s">
         <v>46</v>
-      </c>
-      <c r="D4" s="24" t="n">
-        <v>3</v>
-      </c>
-      <c r="E4" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" s="29" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="24" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" s="29" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -934,4 +1068,186 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:L52"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="8" min="1" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="57.417004048583"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.10526315789474"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="34"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="34"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="34"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="34"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="34"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="34"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="34"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="34"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="34"/>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G51" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="H51" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="I51" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="J51" s="33" t="n">
+        <v>3</v>
+      </c>
+      <c r="K51" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="L51" s="30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G52" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="H52" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="I52" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="J52" s="33" t="n">
+        <v>1</v>
+      </c>
+      <c r="K52" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="L52" s="30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:J9"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>